<commit_message>
dangtq sửa thong tin user
</commit_message>
<xml_diff>
--- a/Business/Trao đổi với khách hàng/Thông tin trao đổi.xlsx
+++ b/Business/Trao đổi với khách hàng/Thông tin trao đổi.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Working\Legaltech\Business\Khách hàng gửi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Working\Legaltech\Business\Trao đổi với khách hàng\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08CAD762-4853-459C-AF11-C698A897ADC6}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{042B39CA-0C4A-492E-84C4-CCE0FC152F65}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -335,7 +335,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -345,6 +345,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -430,7 +436,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -483,6 +489,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -495,27 +522,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
@@ -859,7 +867,7 @@
   <dimension ref="A2:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -938,7 +946,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="31" t="s">
         <v>59</v>
       </c>
       <c r="B6" s="14" t="s">
@@ -951,7 +959,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="31" t="s">
         <v>57</v>
       </c>
       <c r="B7" s="14" t="s">
@@ -1143,7 +1151,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="31" t="s">
         <v>50</v>
       </c>
       <c r="B18" s="14" t="s">
@@ -1156,7 +1164,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="31" t="s">
         <v>20</v>
       </c>
       <c r="B19" s="14" t="s">
@@ -1169,7 +1177,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="31" t="s">
         <v>53</v>
       </c>
       <c r="B20" s="14" t="s">
@@ -1182,7 +1190,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="31" t="s">
         <v>55</v>
       </c>
       <c r="B21" s="14" t="s">
@@ -1195,7 +1203,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="32" t="s">
         <v>69</v>
       </c>
       <c r="B22" s="14" t="s">
@@ -1208,7 +1216,7 @@
       <c r="E22" s="17"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="32" t="s">
         <v>68</v>
       </c>
       <c r="B23" s="14" t="s">
@@ -1256,25 +1264,25 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
     </row>
     <row r="3" spans="1:6" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
     </row>
     <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -1304,31 +1312,31 @@
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
     </row>
     <row r="7" spans="1:6" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
     </row>
     <row r="8" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
     </row>
     <row r="9" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
@@ -1350,23 +1358,23 @@
       <c r="A10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
     </row>
     <row r="11" spans="1:6" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
     </row>
     <row r="12" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
@@ -1385,48 +1393,48 @@
       <c r="F12" s="7"/>
     </row>
     <row r="13" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
     </row>
     <row r="14" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>23</v>
       </c>
       <c r="B14" s="11"/>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
     </row>
     <row r="15" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
         <v>25</v>
       </c>
       <c r="B15" s="7"/>
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
     </row>
     <row r="16" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="30"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
     </row>
     <row r="17" spans="1:6" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
@@ -1454,17 +1462,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="A16:F16"/>
     <mergeCell ref="B10:F10"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B6:F6"/>
     <mergeCell ref="B7:F7"/>
     <mergeCell ref="A8:F8"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="A16:F16"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B10" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
dangtq them don 3d
</commit_message>
<xml_diff>
--- a/Business/Trao đổi với khách hàng/Thông tin trao đổi.xlsx
+++ b/Business/Trao đổi với khách hàng/Thông tin trao đổi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Working\Legaltech\Business\Trao đổi với khách hàng\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CCAA747-A905-4190-A44A-9DAA1B62470E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F735F82C-730A-4CF0-B777-F272AD80BD4D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="thông tin người dùng" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="58">
   <si>
     <t>Email</t>
   </si>
@@ -195,6 +195,12 @@
   </si>
   <si>
     <t>Mã khách hàng</t>
+  </si>
+  <si>
+    <t>3d</t>
+  </si>
+  <si>
+    <t>\Business\Application forms\3d_Request for appeal</t>
   </si>
 </sst>
 </file>
@@ -316,16 +322,16 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -668,7 +674,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{979A9DB1-D662-4145-823D-4403505B585A}">
   <dimension ref="A2:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A21" sqref="A19:B21"/>
     </sheetView>
   </sheetViews>
@@ -789,11 +795,11 @@
       <c r="E8" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -811,9 +817,9 @@
       <c r="E9" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -831,9 +837,9 @@
       <c r="E10" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -851,9 +857,9 @@
       <c r="E11" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -869,9 +875,9 @@
       <c r="E12" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -887,9 +893,9 @@
       <c r="E13" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -903,9 +909,9 @@
       <c r="E14" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -919,9 +925,9 @@
       <c r="E15" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -935,9 +941,9 @@
       <c r="E16" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
@@ -1031,13 +1037,13 @@
       <c r="E23" s="4"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="E24" s="15" t="s">
+      <c r="E24" s="13" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1052,9 +1058,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09B71920-8BBE-4A16-AA07-E65967DEC3F5}">
-  <dimension ref="A3:D7"/>
+  <dimension ref="A3:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -1127,6 +1133,20 @@
         <v>52</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="10">
+        <v>43264</v>
+      </c>
+      <c r="D8" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>